<commit_message>
Add case for R742001001
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-LISTSWS/MS-LISTSWS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-LISTSWS/MS-LISTSWS_RequirementSpecification.xlsx
@@ -16924,19 +16924,19 @@
     <t>Verified by derived requirements: MS-LISTSWS_R742001001.</t>
   </si>
   <si>
-    <t>MS-LISTSWS_R976:I, MS-LISTSWS_R976001001</t>
-  </si>
-  <si>
-    <t>MS-LISTSWS_R976001001</t>
-  </si>
-  <si>
-    <t>[In Appendix B: Product Behavior] Implementation does not return the filed when the filed  referenced in a FieldRef element of viewFields has no value filled.</t>
-  </si>
-  <si>
     <t>Implementation does not return to the client, when the client attempts to open files asynchronously from the server. (SharePoint Foundation 2010 follows this behavior.)</t>
   </si>
   <si>
     <t>Implementation does return to the client, when the client attempts to open files asynchronously from the server.&lt;8&gt;Section 2.2.4.11:  This attribute is returned by SharePoint Foundation 2013. (SharePoint Foundation 2013 and SharePoint Server 2016 follow this behavior.)</t>
+  </si>
+  <si>
+    <t>MS-LISTSWS_R976:I,LISTSWS_R742001:i</t>
+  </si>
+  <si>
+    <t>MS-LISTSWS_R742001001</t>
+  </si>
+  <si>
+    <t>[In Appendix B: Product Behavior] Implementation does not return the filed when the filed  referenced in a FieldRef element of viewFields has no value filled. (SharePoint Foundation 2010 and above follow this behavior.)</t>
   </si>
 </sst>
 </file>
@@ -17214,6 +17214,30 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -17238,183 +17262,11 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
+  <dxfs count="27">
     <dxf>
       <font>
         <b val="0"/>
@@ -17753,6 +17605,50 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -17882,34 +17778,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I2238" tableType="xml" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I2238" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
   <autoFilter ref="A19:I2238"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="44">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="43">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="42">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="41">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="40">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="39">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="38">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="37">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="36">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -17918,12 +17814,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32" totalsRowBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="30"/>
-    <tableColumn id="2" name="Test" dataDxfId="29"/>
-    <tableColumn id="3" name="Description" dataDxfId="28"/>
+    <tableColumn id="1" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -18219,8 +18115,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L2240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2027" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2031" sqref="C2031"/>
+    <sheetView tabSelected="1" topLeftCell="A2231" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2233" sqref="C2233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -18275,127 +18171,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -18408,12 +18304,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -18426,12 +18322,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -18444,12 +18340,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -18462,60 +18358,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -69146,7 +69042,7 @@
         <v>2493</v>
       </c>
       <c r="C2031" s="20" t="s">
-        <v>4897</v>
+        <v>4894</v>
       </c>
       <c r="D2031" s="30" t="s">
         <v>4770</v>
@@ -69173,7 +69069,7 @@
         <v>2493</v>
       </c>
       <c r="C2032" s="20" t="s">
-        <v>4896</v>
+        <v>4893</v>
       </c>
       <c r="D2032" s="30" t="s">
         <v>4770</v>
@@ -74934,18 +74830,18 @@
         <v>4530</v>
       </c>
     </row>
-    <row r="2237" spans="1:9" ht="30">
+    <row r="2237" spans="1:9" ht="45">
       <c r="A2237" s="22" t="s">
-        <v>4894</v>
-      </c>
-      <c r="B2237" s="47" t="s">
+        <v>4896</v>
+      </c>
+      <c r="B2237" s="34" t="s">
         <v>2493</v>
       </c>
-      <c r="C2237" s="48" t="s">
+      <c r="C2237" s="35" t="s">
+        <v>4897</v>
+      </c>
+      <c r="D2237" s="33" t="s">
         <v>4895</v>
-      </c>
-      <c r="D2237" s="46" t="s">
-        <v>4893</v>
       </c>
       <c r="E2237" s="30" t="s">
         <v>22</v>
@@ -74953,13 +74849,13 @@
       <c r="F2237" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G2237" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2237" s="46" t="s">
+      <c r="G2237" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2237" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="I2237" s="48"/>
+      <c r="I2237" s="35"/>
     </row>
     <row r="2238" spans="1:9" ht="105">
       <c r="A2238" s="30" t="s">
@@ -74996,11 +74892,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -75008,35 +74899,40 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:H141 I20:I1338 A34:I2238">
-    <cfRule type="expression" dxfId="27" priority="53">
+    <cfRule type="expression" dxfId="26" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="54">
+    <cfRule type="expression" dxfId="25" priority="54">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="61">
+    <cfRule type="expression" dxfId="24" priority="61">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:H141 I20:I1338 A34:I2238">
-    <cfRule type="expression" dxfId="24" priority="7">
+    <cfRule type="expression" dxfId="23" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="8">
+    <cfRule type="expression" dxfId="22" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="9">
+    <cfRule type="expression" dxfId="21" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F2238">
-    <cfRule type="expression" dxfId="21" priority="13">
+    <cfRule type="expression" dxfId="20" priority="13">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="14">
+    <cfRule type="expression" dxfId="19" priority="14">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -75074,6 +74970,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -75122,32 +75033,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -75161,15 +75056,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
MS-LISTSWS: update RS742001001 and 1401001
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-LISTSWS/MS-LISTSWS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-LISTSWS/MS-LISTSWS_RequirementSpecification.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16061" uniqueCount="4898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16062" uniqueCount="4898">
   <si>
     <t>Req ID</t>
   </si>
@@ -16936,7 +16936,7 @@
     <t>MS-LISTSWS_R742001001</t>
   </si>
   <si>
-    <t>[In Appendix B: Product Behavior] Implementation does not return the filed when the filed  referenced in a FieldRef element of viewFields has no value filled. (SharePoint Foundation 2010 and above follow this behavior.)</t>
+    <t>[In Appendix B: Product Behavior] Implementation does not return the filed when the filed  referenced in a FieldRef element of viewFields has no value filled. (Windows SharePoint Services 3.0 and above follow this behavior.)</t>
   </si>
 </sst>
 </file>
@@ -17223,21 +17223,6 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -17262,11 +17247,56 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="33">
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -17778,34 +17808,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I2238" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I2238" tableType="xml" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" connectionId="1">
   <autoFilter ref="A19:I2238"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="22">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="21">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="20">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="19">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="18">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="17">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -17814,12 +17844,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="2"/>
-    <tableColumn id="2" name="Test" dataDxfId="1"/>
-    <tableColumn id="3" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" name="Scope" dataDxfId="8"/>
+    <tableColumn id="2" name="Test" dataDxfId="7"/>
+    <tableColumn id="3" name="Description" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -18115,8 +18145,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L2240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2231" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2233" sqref="C2233"/>
+    <sheetView tabSelected="1" topLeftCell="D2232" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I2237" sqref="I2237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -18171,127 +18201,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -18304,12 +18334,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -18322,12 +18352,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -18340,12 +18370,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -18358,60 +18388,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -24935,7 +24965,7 @@
       <c r="B279" s="31" t="s">
         <v>2254</v>
       </c>
-      <c r="C279" s="32" t="s">
+      <c r="C279" s="20" t="s">
         <v>4581</v>
       </c>
       <c r="D279" s="30"/>
@@ -74855,7 +74885,9 @@
       <c r="H2237" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="I2237" s="35"/>
+      <c r="I2237" s="32" t="s">
+        <v>4530</v>
+      </c>
     </row>
     <row r="2238" spans="1:9" ht="105">
       <c r="A2238" s="30" t="s">
@@ -74892,6 +74924,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -74899,40 +74936,35 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:H141 I20:I1338 A34:I2238">
-    <cfRule type="expression" dxfId="26" priority="53">
+    <cfRule type="expression" dxfId="32" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="54">
+    <cfRule type="expression" dxfId="31" priority="54">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="61">
+    <cfRule type="expression" dxfId="30" priority="61">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:H141 I20:I1338 A34:I2238">
-    <cfRule type="expression" dxfId="23" priority="7">
+    <cfRule type="expression" dxfId="29" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="8">
+    <cfRule type="expression" dxfId="28" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="9">
+    <cfRule type="expression" dxfId="27" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F2238">
-    <cfRule type="expression" dxfId="20" priority="13">
+    <cfRule type="expression" dxfId="26" priority="13">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="14">
+    <cfRule type="expression" dxfId="25" priority="14">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -74970,21 +75002,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -75033,16 +75050,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -75056,16 +75089,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
MS-LISTSWS: Add capture R3010001 and cases R713 R1906
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-LISTSWS/MS-LISTSWS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-LISTSWS/MS-LISTSWS_RequirementSpecification.xlsx
@@ -17223,6 +17223,21 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -17247,56 +17262,11 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
+  <dxfs count="27">
     <dxf>
       <font>
         <b val="0"/>
@@ -17808,34 +17778,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I2238" tableType="xml" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I2238" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
   <autoFilter ref="A19:I2238"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="22">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="21">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="20">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="19">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="18">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="17">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="16">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="15">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="14">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -17844,12 +17814,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="8"/>
-    <tableColumn id="2" name="Test" dataDxfId="7"/>
-    <tableColumn id="3" name="Description" dataDxfId="6"/>
+    <tableColumn id="1" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -18145,9 +18115,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L2240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2232" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2237" sqref="I2237"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -18201,127 +18169,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -18334,12 +18302,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -18352,12 +18320,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -18370,12 +18338,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -18388,60 +18356,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -23554,7 +23522,7 @@
         <v>15</v>
       </c>
       <c r="H222" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I222" s="32"/>
     </row>
@@ -26791,8 +26759,8 @@
       <c r="G350" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="H350" s="30" t="s">
-        <v>21</v>
+      <c r="H350" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="I350" s="32"/>
     </row>
@@ -53779,7 +53747,7 @@
       <c r="B1425" s="31" t="s">
         <v>2429</v>
       </c>
-      <c r="C1425" s="32" t="s">
+      <c r="C1425" s="20" t="s">
         <v>3732</v>
       </c>
       <c r="D1425" s="30"/>
@@ -70145,7 +70113,7 @@
         <v>15</v>
       </c>
       <c r="H2069" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I2069" s="32"/>
     </row>
@@ -74924,11 +74892,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -74936,35 +74899,40 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:H141 I20:I1338 A34:I2238">
-    <cfRule type="expression" dxfId="32" priority="53">
+    <cfRule type="expression" dxfId="26" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="54">
+    <cfRule type="expression" dxfId="25" priority="54">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="61">
+    <cfRule type="expression" dxfId="24" priority="61">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:H141 I20:I1338 A34:I2238">
-    <cfRule type="expression" dxfId="29" priority="7">
+    <cfRule type="expression" dxfId="23" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="8">
+    <cfRule type="expression" dxfId="22" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="9">
+    <cfRule type="expression" dxfId="21" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F2238">
-    <cfRule type="expression" dxfId="26" priority="13">
+    <cfRule type="expression" dxfId="20" priority="13">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="14">
+    <cfRule type="expression" dxfId="19" priority="14">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -75002,6 +74970,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -75050,32 +75033,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -75089,15 +75056,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
MS-LISTSWS: update R3010001 for O14 O15 O16
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-LISTSWS/MS-LISTSWS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-LISTSWS/MS-LISTSWS_RequirementSpecification.xlsx
@@ -17223,21 +17223,6 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -17261,6 +17246,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -18115,7 +18115,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L2240"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A364" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C372" sqref="C372"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -18169,127 +18171,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -18302,12 +18304,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -18320,12 +18322,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -18338,12 +18340,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -18356,60 +18358,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -24908,7 +24910,7 @@
       <c r="B278" s="31" t="s">
         <v>2254</v>
       </c>
-      <c r="C278" s="32" t="s">
+      <c r="C278" s="20" t="s">
         <v>2747</v>
       </c>
       <c r="D278" s="30"/>
@@ -24921,8 +24923,8 @@
       <c r="G278" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="H278" s="30" t="s">
-        <v>21</v>
+      <c r="H278" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="I278" s="32"/>
     </row>
@@ -53585,8 +53587,8 @@
       <c r="G1418" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="H1418" s="30" t="s">
-        <v>20</v>
+      <c r="H1418" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="I1418" s="32"/>
     </row>
@@ -58298,7 +58300,7 @@
       <c r="B1606" s="31" t="s">
         <v>2451</v>
       </c>
-      <c r="C1606" s="32" t="s">
+      <c r="C1606" s="20" t="s">
         <v>4729</v>
       </c>
       <c r="D1606" s="30"/>
@@ -58317,13 +58319,13 @@
       <c r="I1606" s="32"/>
     </row>
     <row r="1607" spans="1:9" ht="60">
-      <c r="A1607" s="30" t="s">
+      <c r="A1607" s="22" t="s">
         <v>4730</v>
       </c>
       <c r="B1607" s="31" t="s">
         <v>2451</v>
       </c>
-      <c r="C1607" s="32" t="s">
+      <c r="C1607" s="20" t="s">
         <v>4731</v>
       </c>
       <c r="D1607" s="30"/>
@@ -74892,6 +74894,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -74899,11 +74906,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:H141 I20:I1338 A34:I2238">
@@ -74970,21 +74972,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -75033,16 +75020,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -75056,16 +75059,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
MS-LISTSWS:Update RS to unverified
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-LISTSWS/MS-LISTSWS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-LISTSWS/MS-LISTSWS_RequirementSpecification.xlsx
@@ -17223,6 +17223,21 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -17246,21 +17261,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -18115,8 +18115,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L2240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A364" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C372" sqref="C372"/>
+    <sheetView tabSelected="1" topLeftCell="D364" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H374" sqref="H374"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -18171,127 +18171,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -18304,12 +18304,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -18322,12 +18322,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -18340,12 +18340,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -18358,60 +18358,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -27340,8 +27340,8 @@
       <c r="G373" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="H373" s="30" t="s">
-        <v>21</v>
+      <c r="H373" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="I373" s="32"/>
     </row>
@@ -27365,8 +27365,8 @@
       <c r="G374" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="H374" s="30" t="s">
-        <v>21</v>
+      <c r="H374" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="I374" s="32"/>
     </row>
@@ -27390,8 +27390,8 @@
       <c r="G375" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="H375" s="30" t="s">
-        <v>21</v>
+      <c r="H375" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="I375" s="32"/>
     </row>
@@ -38091,8 +38091,8 @@
       <c r="G802" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="H802" s="30" t="s">
-        <v>20</v>
+      <c r="H802" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="I802" s="32"/>
     </row>
@@ -53337,8 +53337,8 @@
       <c r="G1408" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="H1408" s="30" t="s">
-        <v>20</v>
+      <c r="H1408" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="I1408" s="32"/>
     </row>
@@ -62077,8 +62077,8 @@
       <c r="G1756" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="H1756" s="30" t="s">
-        <v>21</v>
+      <c r="H1756" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="I1756" s="32"/>
     </row>
@@ -74894,11 +74894,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -74906,6 +74901,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:H141 I20:I1338 A34:I2238">
@@ -74972,6 +74972,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -75020,32 +75035,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -75059,15 +75058,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
MS-LISTSWS: Update RS file for R1977001
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-LISTSWS/MS-LISTSWS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-LISTSWS/MS-LISTSWS_RequirementSpecification.xlsx
@@ -17223,21 +17223,6 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -17261,6 +17246,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -18115,13 +18115,13 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L2240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1401" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1409" sqref="C1409"/>
+    <sheetView tabSelected="1" topLeftCell="D1601" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H1609" sqref="H1609"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
     <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
@@ -18171,127 +18171,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -18304,12 +18304,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -18322,12 +18322,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -18340,12 +18340,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -18358,60 +18358,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -58275,7 +58275,7 @@
       <c r="B1605" s="31" t="s">
         <v>2451</v>
       </c>
-      <c r="C1605" s="32" t="s">
+      <c r="C1605" s="20" t="s">
         <v>4728</v>
       </c>
       <c r="D1605" s="30"/>
@@ -58336,10 +58336,10 @@
         <v>6</v>
       </c>
       <c r="G1607" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H1607" s="22" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I1607" s="32"/>
     </row>
@@ -74894,6 +74894,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -74901,11 +74906,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:H141 I20:I1338 A34:I2238">
@@ -74972,21 +74972,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -75035,16 +75020,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -75058,16 +75059,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add capture code and test cases for new attributes in ListDefinitionCT.
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-LISTSWS/MS-LISTSWS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-LISTSWS/MS-LISTSWS_RequirementSpecification.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9233F8-9132-4F90-B37E-D8D1E19EF12B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04863DC-0B03-4175-8E41-7390212E0043}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16205" uniqueCount="4957">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16205" uniqueCount="4958">
   <si>
     <t>Req ID</t>
   </si>
@@ -17403,6 +17403,10 @@
 	  &lt;s:attribute name="RootFolderId" type="s:string" use="optional"/&gt;
 	  &lt;s:attribute name="IrmSyncable" type="core:TRUEFALSE" use="optional"/&gt;/&gt;
 	&lt;/s:complexType&gt; </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS-LISTSWS_R542000102</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -17691,6 +17695,21 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -17714,21 +17733,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -18671,127 +18675,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -18804,12 +18808,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -18822,12 +18826,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -18840,12 +18844,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -18858,60 +18862,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -70543,7 +70547,7 @@
     </row>
     <row r="2068" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2068" s="22" t="s">
-        <v>4747</v>
+        <v>4957</v>
       </c>
       <c r="B2068" s="24" t="s">
         <v>4745</v>
@@ -75876,11 +75880,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -75888,6 +75887,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:H141 I20:I310 A34:I2256">
@@ -75954,6 +75958,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -76002,32 +76021,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -76041,15 +76044,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add TDI 1518047 related property in SHOULDMAY file
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-LISTSWS/MS-LISTSWS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-LISTSWS/MS-LISTSWS_RequirementSpecification.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96987DB-E893-4235-9009-5B64CA78C96B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6568204C-7B15-4D02-84A8-AA418DCDA042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="1305" windowWidth="25890" windowHeight="12480" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="25890" windowHeight="12480" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -17687,21 +17687,6 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -17725,6 +17710,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -18613,8 +18613,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L2264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A313" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H323" sqref="H323"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -18669,127 +18669,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48"/>
-      <c r="I10" s="48"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -18802,12 +18802,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="44"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -18820,12 +18820,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -18838,12 +18838,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="45"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -18856,60 +18856,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="46"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="43"/>
-      <c r="I16" s="43"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="50"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -26481,7 +26481,7 @@
         <v>15</v>
       </c>
       <c r="H319" s="36" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I319" s="37"/>
     </row>
@@ -26581,7 +26581,7 @@
         <v>15</v>
       </c>
       <c r="H323" s="36" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I323" s="37"/>
     </row>
@@ -76026,6 +76026,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -76033,11 +76038,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:H141 I20:I310 A34:I2262">
@@ -76104,12 +76104,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -76162,15 +76159,24 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -76191,15 +76197,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>